<commit_message>
Add all reduce results for P100.
</commit_message>
<xml_diff>
--- a/results/DeepBench_NV_P100.xlsx
+++ b/results/DeepBench_NV_P100.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="77">
   <si>
     <t>Dense Matrix Multiplication</t>
   </si>
@@ -218,6 +218,39 @@
   </si>
   <si>
     <t>IMPLICIT_GEMM</t>
+  </si>
+  <si>
+    <t>All-Reduce</t>
+  </si>
+  <si>
+    <t>Size # floats</t>
+  </si>
+  <si>
+    <t># chips / accelerator cards</t>
+  </si>
+  <si>
+    <t>Mean All Reduce Time (msec)</t>
+  </si>
+  <si>
+    <t>Gigabytes/sec</t>
+  </si>
+  <si>
+    <t>Selected Algorithm</t>
+  </si>
+  <si>
+    <t>Std Dev All Reduce Time (msec)</t>
+  </si>
+  <si>
+    <t>NCCL Single Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSU MPI </t>
+  </si>
+  <si>
+    <t>OSU MPI</t>
+  </si>
+  <si>
+    <t>NCCL MPI</t>
   </si>
 </sst>
 </file>
@@ -1228,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE172"/>
+  <dimension ref="A1:AE199"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A172" sqref="A172"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2456,7 +2489,7 @@
         <v>19.658999999999999</v>
       </c>
       <c r="J48" s="2">
-        <f>(2*C48*D48*E48)/(I48/1000)/10^12</f>
+        <f t="shared" ref="J48:J63" si="1">(2*C48*D48*E48)/(I48/1000)/10^12</f>
         <v>8.3709671661834282</v>
       </c>
       <c r="K48" s="2"/>
@@ -2482,7 +2515,7 @@
         <v>0.47399999999999998</v>
       </c>
       <c r="J49" s="2">
-        <f>(2*C49*D49*E49)/(I49/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>2.1981063291139242</v>
       </c>
       <c r="K49" s="2"/>
@@ -2508,7 +2541,7 @@
         <v>22.468</v>
       </c>
       <c r="J50" s="2">
-        <f>(2*C50*D50*E50)/(I50/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>8.5229497995371197</v>
       </c>
       <c r="K50" s="2"/>
@@ -2534,7 +2567,7 @@
         <v>0.43</v>
       </c>
       <c r="J51" s="2">
-        <f>(2*C51*D51*E51)/(I51/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>2.8195244651162792</v>
       </c>
       <c r="K51" s="2"/>
@@ -2560,7 +2593,7 @@
         <v>28.332999999999998</v>
       </c>
       <c r="J52" s="2">
-        <f>(2*C52*D52*E52)/(I52/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>8.4483480436240441</v>
       </c>
       <c r="K52" s="2"/>
@@ -2586,7 +2619,7 @@
         <v>0.69</v>
       </c>
       <c r="J53" s="2">
-        <f>(2*C53*D53*E53)/(I53/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>2.1963686956521742</v>
       </c>
       <c r="K53" s="2"/>
@@ -2612,7 +2645,7 @@
         <v>45.276000000000003</v>
       </c>
       <c r="J54" s="2">
-        <f>(2*C54*D54*E54)/(I54/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>8.4589467309833015</v>
       </c>
       <c r="K54" s="2"/>
@@ -2638,7 +2671,7 @@
         <v>0.79700000000000004</v>
       </c>
       <c r="J55" s="2">
-        <f>(2*C55*D55*E55)/(I55/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>3.0423977917189458</v>
       </c>
       <c r="K55" s="2"/>
@@ -2664,7 +2697,7 @@
         <v>20.073</v>
       </c>
       <c r="J56" s="2">
-        <f>(2*C56*D56*E56)/(I56/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>8.1983183141533402</v>
       </c>
       <c r="K56" s="2"/>
@@ -2690,7 +2723,7 @@
         <v>0.36599999999999999</v>
       </c>
       <c r="J57" s="2">
-        <f>(2*C57*D57*E57)/(I57/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>2.8467278688524589</v>
       </c>
       <c r="K57" s="2"/>
@@ -2716,7 +2749,7 @@
         <v>23.132000000000001</v>
       </c>
       <c r="J58" s="2">
-        <f>(2*C58*D58*E58)/(I58/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>8.278300021442158</v>
       </c>
       <c r="K58" s="2"/>
@@ -2742,7 +2775,7 @@
         <v>0.42</v>
       </c>
       <c r="J59" s="2">
-        <f>(2*C59*D59*E59)/(I59/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>2.8866560000000003</v>
       </c>
       <c r="K59" s="2"/>
@@ -2768,7 +2801,7 @@
         <v>29.146999999999998</v>
       </c>
       <c r="J60" s="2">
-        <f>(2*C60*D60*E60)/(I60/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>8.2124076275431435</v>
       </c>
       <c r="K60" s="2"/>
@@ -2794,7 +2827,7 @@
         <v>0.51600000000000001</v>
       </c>
       <c r="J61" s="2">
-        <f>(2*C61*D61*E61)/(I61/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>2.9370046511627912</v>
       </c>
       <c r="K61" s="2"/>
@@ -2820,7 +2853,7 @@
         <v>45.896000000000001</v>
       </c>
       <c r="J62" s="2">
-        <f>(2*C62*D62*E62)/(I62/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>8.344676490151647</v>
       </c>
       <c r="K62" s="2"/>
@@ -2846,7 +2879,7 @@
         <v>0.79300000000000004</v>
       </c>
       <c r="J63" s="2">
-        <f>(2*C63*D63*E63)/(I63/1000)/10^12</f>
+        <f t="shared" si="1"/>
         <v>3.0577440605296338</v>
       </c>
       <c r="K63" s="2"/>
@@ -2878,7 +2911,7 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="J65" s="2">
-        <f>(2*C65*D65*E65)/(I65/1000)/10^12</f>
+        <f t="shared" ref="J65:J80" si="2">(2*C65*D65*E65)/(I65/1000)/10^12</f>
         <v>1.1983725714285713</v>
       </c>
       <c r="K65" s="2"/>
@@ -2904,7 +2937,7 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="J66" s="2">
-        <f>(2*C66*D66*E66)/(I66/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>3.0916245700245701</v>
       </c>
       <c r="K66" s="2"/>
@@ -2930,7 +2963,7 @@
         <v>0.504</v>
       </c>
       <c r="J67" s="2">
-        <f>(2*C67*D67*E67)/(I67/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>4.9932190476190481</v>
       </c>
       <c r="K67" s="2"/>
@@ -2956,7 +2989,7 @@
         <v>1.0620000000000001</v>
       </c>
       <c r="J68" s="2">
-        <f>(2*C68*D68*E68)/(I68/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>4.7393265536723161</v>
       </c>
       <c r="K68" s="2"/>
@@ -2982,7 +3015,7 @@
         <v>0.45600000000000002</v>
       </c>
       <c r="J69" s="2">
-        <f>(2*C69*D69*E69)/(I69/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>1.3797052631578948</v>
       </c>
       <c r="K69" s="2"/>
@@ -3008,7 +3041,7 @@
         <v>0.51400000000000001</v>
       </c>
       <c r="J70" s="2">
-        <f>(2*C70*D70*E70)/(I70/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>2.4480373540856029</v>
       </c>
       <c r="K70" s="2"/>
@@ -3034,7 +3067,7 @@
         <v>0.51500000000000001</v>
       </c>
       <c r="J71" s="2">
-        <f>(2*C71*D71*E71)/(I71/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>4.8865677669902912</v>
       </c>
       <c r="K71" s="2"/>
@@ -3060,7 +3093,7 @@
         <v>1.0880000000000001</v>
       </c>
       <c r="J72" s="2">
-        <f>(2*C72*D72*E72)/(I72/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>4.6260705882352937</v>
       </c>
       <c r="K72" s="2"/>
@@ -3087,7 +3120,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="J73" s="2">
-        <f>(2*C73*D73*E73)/(I73/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>1.6236015483870967</v>
       </c>
       <c r="K73" s="2"/>
@@ -3095,7 +3128,7 @@
     </row>
     <row r="74" spans="3:12">
       <c r="C74">
-        <f t="shared" ref="C74:C80" si="1">3*1024</f>
+        <f t="shared" ref="C74:C80" si="3">3*1024</f>
         <v>3072</v>
       </c>
       <c r="D74">
@@ -3114,7 +3147,7 @@
         <v>0.153</v>
       </c>
       <c r="J74" s="2">
-        <f>(2*C74*D74*E74)/(I74/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>1.3158600784313725</v>
       </c>
       <c r="K74" s="2"/>
@@ -3122,7 +3155,7 @@
     </row>
     <row r="75" spans="3:12">
       <c r="C75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3072</v>
       </c>
       <c r="D75">
@@ -3141,7 +3174,7 @@
         <v>0.109</v>
       </c>
       <c r="J75" s="2">
-        <f>(2*C75*D75*E75)/(I75/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>3.694065908256881</v>
       </c>
       <c r="K75" s="2"/>
@@ -3149,7 +3182,7 @@
     </row>
     <row r="76" spans="3:12">
       <c r="C76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3072</v>
       </c>
       <c r="D76">
@@ -3168,7 +3201,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="J76" s="2">
-        <f>(2*C76*D76*E76)/(I76/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>5.6315130629370636</v>
       </c>
       <c r="K76" s="2"/>
@@ -3176,7 +3209,7 @@
     </row>
     <row r="77" spans="3:12">
       <c r="C77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3072</v>
       </c>
       <c r="D77">
@@ -3195,7 +3228,7 @@
         <v>0.109</v>
       </c>
       <c r="J77" s="2">
-        <f>(2*C77*D77*E77)/(I77/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>0.92351647706422024</v>
       </c>
       <c r="K77" s="2"/>
@@ -3203,7 +3236,7 @@
     </row>
     <row r="78" spans="3:12">
       <c r="C78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3072</v>
       </c>
       <c r="D78">
@@ -3222,7 +3255,7 @@
         <v>0.15</v>
       </c>
       <c r="J78" s="2">
-        <f>(2*C78*D78*E78)/(I78/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>1.34217728</v>
       </c>
       <c r="K78" s="2"/>
@@ -3230,7 +3263,7 @@
     </row>
     <row r="79" spans="3:12">
       <c r="C79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3072</v>
       </c>
       <c r="D79">
@@ -3249,7 +3282,7 @@
         <v>0.12</v>
       </c>
       <c r="J79" s="2">
-        <f>(2*C79*D79*E79)/(I79/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>3.3554432000000003</v>
       </c>
       <c r="K79" s="2"/>
@@ -3257,7 +3290,7 @@
     </row>
     <row r="80" spans="3:12">
       <c r="C80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3072</v>
       </c>
       <c r="D80">
@@ -3276,7 +3309,7 @@
         <v>0.151</v>
       </c>
       <c r="J80" s="2">
-        <f>(2*C80*D80*E80)/(I80/1000)/10^12</f>
+        <f t="shared" si="2"/>
         <v>5.3331547549668876</v>
       </c>
       <c r="K80" s="2"/>
@@ -3457,11 +3490,11 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="R91" s="4">
-        <f t="shared" ref="R91:R126" si="2">(D91-H91+1+2*J91)/L91</f>
+        <f t="shared" ref="R91:R126" si="4">(D91-H91+1+2*J91)/L91</f>
         <v>78.5</v>
       </c>
       <c r="S91" s="4">
-        <f t="shared" ref="S91:S126" si="3">(C91-I91+1+2*K91)/M91</f>
+        <f t="shared" ref="S91:S126" si="5">(C91-I91+1+2*K91)/M91</f>
         <v>340.5</v>
       </c>
       <c r="T91" s="2">
@@ -3529,11 +3562,11 @@
         <v>0.52100000000000002</v>
       </c>
       <c r="R92" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>78.5</v>
       </c>
       <c r="S92" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>340.5</v>
       </c>
       <c r="T92" s="2">
@@ -3541,14 +3574,14 @@
         <v>0.76</v>
       </c>
       <c r="U92" s="2">
-        <f t="shared" ref="U92:U126" si="4">(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(N92/1000)/10^12</f>
+        <f t="shared" ref="U92:U126" si="6">(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(N92/1000)/10^12</f>
         <v>5.7260987447698746</v>
       </c>
       <c r="V92" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W92" s="2">
-        <f t="shared" ref="W92:W126" si="5">(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(P92/1000)/10^12</f>
+        <f t="shared" ref="W92:W126" si="7">(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(P92/1000)/10^12</f>
         <v>2.6267516314779273</v>
       </c>
       <c r="X92" t="s">
@@ -3601,11 +3634,11 @@
         <v>0.98699999999999999</v>
       </c>
       <c r="R93" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>78.5</v>
       </c>
       <c r="S93" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>340.5</v>
       </c>
       <c r="T93" s="2">
@@ -3613,14 +3646,14 @@
         <v>1.446</v>
       </c>
       <c r="U93" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.9631267973856197</v>
       </c>
       <c r="V93" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W93" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.7731258358662614</v>
       </c>
       <c r="X93" t="s">
@@ -3673,11 +3706,11 @@
         <v>1.873</v>
       </c>
       <c r="R94" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>78.5</v>
       </c>
       <c r="S94" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>340.5</v>
       </c>
       <c r="T94" s="2">
@@ -3685,14 +3718,14 @@
         <v>2.7730000000000001</v>
       </c>
       <c r="U94" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.0823893333333343</v>
       </c>
       <c r="V94" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W94" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.9226643886812598</v>
       </c>
       <c r="X94" t="s">
@@ -3745,11 +3778,11 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="R95" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
       <c r="S95" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="T95" s="2">
@@ -3757,15 +3790,15 @@
         <v>2.3359999999999999</v>
       </c>
       <c r="U95" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.3426865671641783</v>
       </c>
       <c r="V95" s="2">
-        <f t="shared" ref="V95:V126" si="6">(2*$R95*$S95*$F95*$G95*$E95*$H95*$I95)/(O95/1000)/10^12</f>
+        <f t="shared" ref="V95:V126" si="8">(2*$R95*$S95*$F95*$G95*$E95*$H95*$I95)/(O95/1000)/10^12</f>
         <v>1.7112483221476509</v>
       </c>
       <c r="W95" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.7427027027027036</v>
       </c>
       <c r="X95" t="s">
@@ -3818,27 +3851,27 @@
         <v>0.84199999999999997</v>
       </c>
       <c r="R96" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
       <c r="S96" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="T96" s="2">
-        <f t="shared" ref="T96:T98" si="7">N96+O96+P96</f>
+        <f t="shared" ref="T96:T98" si="9">N96+O96+P96</f>
         <v>4.6459999999999999</v>
       </c>
       <c r="U96" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.078092967818832</v>
       </c>
       <c r="V96" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.7199055649241148</v>
       </c>
       <c r="W96" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.0564370546318287</v>
       </c>
       <c r="X96" t="s">
@@ -3891,27 +3924,27 @@
         <v>1.6990000000000001</v>
       </c>
       <c r="R97" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
       <c r="S97" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="T97" s="2">
+        <f t="shared" si="9"/>
+        <v>9.1780000000000008</v>
+      </c>
+      <c r="U97" s="2">
+        <f t="shared" si="6"/>
+        <v>6.9952263374485604</v>
+      </c>
+      <c r="V97" s="2">
+        <f t="shared" si="8"/>
+        <v>1.6939113104135526</v>
+      </c>
+      <c r="W97" s="2">
         <f t="shared" si="7"/>
-        <v>9.1780000000000008</v>
-      </c>
-      <c r="U97" s="2">
-        <f t="shared" si="4"/>
-        <v>6.9952263374485604</v>
-      </c>
-      <c r="V97" s="2">
-        <f t="shared" si="6"/>
-        <v>1.6939113104135526</v>
-      </c>
-      <c r="W97" s="2">
-        <f t="shared" si="5"/>
         <v>6.0029664508534433</v>
       </c>
       <c r="X97" t="s">
@@ -3964,27 +3997,27 @@
         <v>3.3650000000000002</v>
       </c>
       <c r="R98" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
       <c r="S98" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="T98" s="2">
+        <f t="shared" si="9"/>
+        <v>18.133000000000003</v>
+      </c>
+      <c r="U98" s="2">
+        <f t="shared" si="6"/>
+        <v>7.2565208110992527</v>
+      </c>
+      <c r="V98" s="2">
+        <f t="shared" si="8"/>
+        <v>1.7059529982437065</v>
+      </c>
+      <c r="W98" s="2">
         <f t="shared" si="7"/>
-        <v>18.133000000000003</v>
-      </c>
-      <c r="U98" s="2">
-        <f t="shared" si="4"/>
-        <v>7.2565208110992527</v>
-      </c>
-      <c r="V98" s="2">
-        <f t="shared" si="6"/>
-        <v>1.7059529982437065</v>
-      </c>
-      <c r="W98" s="2">
-        <f t="shared" si="5"/>
         <v>6.0618365527488844</v>
       </c>
       <c r="X98" t="s">
@@ -4037,11 +4070,11 @@
         <v>0.443</v>
       </c>
       <c r="R99" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="S99" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>480</v>
       </c>
       <c r="T99" s="2">
@@ -4049,14 +4082,14 @@
         <v>0.56899999999999995</v>
       </c>
       <c r="U99" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.84260571428571418</v>
       </c>
       <c r="V99" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W99" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.23965760722347632</v>
       </c>
       <c r="X99" t="s">
@@ -4109,11 +4142,11 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="R100" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="S100" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>240</v>
       </c>
       <c r="T100" s="2">
@@ -4121,15 +4154,15 @@
         <v>0.70599999999999996</v>
       </c>
       <c r="U100" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.6623104000000009</v>
       </c>
       <c r="V100" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.2046859405940591</v>
       </c>
       <c r="W100" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.3992840677966103</v>
       </c>
       <c r="X100" t="s">
@@ -4182,27 +4215,27 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="R101" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="S101" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
       <c r="T101" s="2">
-        <f t="shared" ref="T101:T102" si="8">N101+O101+P101</f>
+        <f t="shared" ref="T101:T102" si="10">N101+O101+P101</f>
         <v>0.50800000000000001</v>
       </c>
       <c r="U101" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.3856222608695656</v>
       </c>
       <c r="V101" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.792170275229358</v>
       </c>
       <c r="W101" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.990656901408451</v>
       </c>
       <c r="X101" t="s">
@@ -4255,27 +4288,27 @@
         <v>0.191</v>
       </c>
       <c r="R102" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="S102" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="T102" s="2">
+        <f t="shared" si="10"/>
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="U102" s="2">
+        <f t="shared" si="6"/>
+        <v>7.9378183177570101</v>
+      </c>
+      <c r="V102" s="2">
         <f t="shared" si="8"/>
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="U102" s="2">
-        <f t="shared" si="4"/>
-        <v>7.9378183177570101</v>
-      </c>
-      <c r="V102" s="2">
-        <f t="shared" si="6"/>
         <v>8.5792581818181812</v>
       </c>
       <c r="W102" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.446840628272251</v>
       </c>
       <c r="X102" t="s">
@@ -4328,11 +4361,11 @@
         <v>0.122</v>
       </c>
       <c r="R103" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="S103" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>54</v>
       </c>
       <c r="T103" s="2">
@@ -4340,14 +4373,14 @@
         <v>0.158</v>
       </c>
       <c r="U103" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.2394880000000006</v>
       </c>
       <c r="V103" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W103" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.66083252459016395</v>
       </c>
       <c r="X103" t="s">
@@ -4400,11 +4433,11 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="R104" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="S104" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>54</v>
       </c>
       <c r="T104" s="2">
@@ -4412,15 +4445,15 @@
         <v>0.82399999999999995</v>
       </c>
       <c r="U104" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.4310136470588226</v>
       </c>
       <c r="V104" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8.3898867512195121</v>
       </c>
       <c r="W104" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.1444018891566268</v>
       </c>
       <c r="X104" t="s">
@@ -4473,27 +4506,27 @@
         <v>0.16900000000000001</v>
       </c>
       <c r="R105" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="S105" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="T105" s="2">
-        <f t="shared" ref="T105:T107" si="9">N105+O105+P105</f>
+        <f t="shared" ref="T105:T107" si="11">N105+O105+P105</f>
         <v>0.51600000000000001</v>
       </c>
       <c r="U105" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.8846366896551725</v>
       </c>
       <c r="V105" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9.9417733179190755</v>
       </c>
       <c r="W105" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10.177081562130176</v>
       </c>
       <c r="X105" t="s">
@@ -4546,27 +4579,27 @@
         <v>0.122</v>
       </c>
       <c r="R106" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="S106" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="T106" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.316</v>
       </c>
       <c r="U106" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.2484403200000003</v>
       </c>
       <c r="V106" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9.8387662978723416</v>
       </c>
       <c r="W106" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.5806887868852462</v>
       </c>
       <c r="X106" t="s">
@@ -4619,27 +4652,27 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="R107" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="S107" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="T107" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.623</v>
       </c>
       <c r="U107" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.8535168000000004</v>
       </c>
       <c r="V107" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.2619540645161296</v>
       </c>
       <c r="W107" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.5713495903614465</v>
       </c>
       <c r="X107" t="s">
@@ -4692,11 +4725,11 @@
         <v>0.88300000000000001</v>
       </c>
       <c r="R108" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>224</v>
       </c>
       <c r="S108" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>224</v>
       </c>
       <c r="T108" s="2">
@@ -4704,14 +4737,14 @@
         <v>1.22</v>
       </c>
       <c r="U108" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.1165164629080113</v>
       </c>
       <c r="V108" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W108" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.5710827270668177</v>
       </c>
       <c r="X108" t="s">
@@ -4764,11 +4797,11 @@
         <v>1.905</v>
       </c>
       <c r="R109" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>112</v>
       </c>
       <c r="S109" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
       <c r="T109" s="2">
@@ -4776,15 +4809,15 @@
         <v>4.1950000000000003</v>
       </c>
       <c r="U109" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12.229342571900828</v>
       </c>
       <c r="V109" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>13.701393066666666</v>
       </c>
       <c r="W109" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.7677189039370074</v>
       </c>
       <c r="X109" t="s">
@@ -4838,27 +4871,27 @@
         <v>0.84499999999999997</v>
       </c>
       <c r="R110" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="S110" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="T110" s="2">
-        <f t="shared" ref="T110:T113" si="10">N110+O110+P110</f>
+        <f t="shared" ref="T110:T113" si="12">N110+O110+P110</f>
         <v>3.1109999999999998</v>
       </c>
       <c r="U110" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12.519039350253809</v>
       </c>
       <c r="V110" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>13.650834420664205</v>
       </c>
       <c r="W110" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>17.511839659171599</v>
       </c>
       <c r="X110" t="s">
@@ -4912,27 +4945,27 @@
         <v>0.70199999999999996</v>
       </c>
       <c r="R111" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="S111" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="T111" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.9059999999999997</v>
       </c>
       <c r="U111" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>13.129995130434784</v>
       </c>
       <c r="V111" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>13.739558506963787</v>
       </c>
       <c r="W111" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>21.079066256410258</v>
       </c>
       <c r="X111" t="s">
@@ -4985,27 +5018,27 @@
         <v>0.52</v>
       </c>
       <c r="R112" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="S112" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="T112" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.7010000000000001</v>
       </c>
       <c r="U112" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12.434877741176473</v>
       </c>
       <c r="V112" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>12.625857092150172</v>
       </c>
       <c r="W112" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>14.228369723076922</v>
       </c>
       <c r="X112" t="s">
@@ -5058,27 +5091,27 @@
         <v>0.27700000000000002</v>
       </c>
       <c r="R113" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="S113" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="T113" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.1680000000000001</v>
       </c>
       <c r="U113" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.1104179199999997</v>
       </c>
       <c r="V113" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.1943039999999998</v>
       </c>
       <c r="W113" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.6775742382671472</v>
       </c>
       <c r="X113" t="s">
@@ -5131,11 +5164,11 @@
         <v>1.746</v>
       </c>
       <c r="R114" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>224</v>
       </c>
       <c r="S114" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>224</v>
       </c>
       <c r="T114" s="2">
@@ -5143,14 +5176,14 @@
         <v>2.3980000000000001</v>
       </c>
       <c r="U114" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.255417325153374</v>
       </c>
       <c r="V114" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W114" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.5890790927835052</v>
       </c>
       <c r="X114" t="s">
@@ -5203,11 +5236,11 @@
         <v>3.7330000000000001</v>
       </c>
       <c r="R115" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>112</v>
       </c>
       <c r="S115" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
       <c r="T115" s="2">
@@ -5215,15 +5248,15 @@
         <v>8.1560000000000006</v>
       </c>
       <c r="U115" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12.734513349397591</v>
       </c>
       <c r="V115" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>14.099575523582658</v>
       </c>
       <c r="W115" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.9279424120010713</v>
       </c>
       <c r="X115" t="s">
@@ -5277,27 +5310,27 @@
         <v>1.6080000000000001</v>
       </c>
       <c r="R116" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="S116" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="T116" s="2">
-        <f t="shared" ref="T116:T119" si="11">N116+O116+P116</f>
+        <f t="shared" ref="T116:T119" si="13">N116+O116+P116</f>
         <v>4.74</v>
       </c>
       <c r="U116" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>18.578160090395482</v>
       </c>
       <c r="V116" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.230025356725143</v>
       </c>
       <c r="W116" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.404856358208953</v>
       </c>
       <c r="X116" t="s">
@@ -5351,27 +5384,27 @@
         <v>1.3320000000000001</v>
       </c>
       <c r="R117" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="S117" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="T117" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.0490000000000004</v>
       </c>
       <c r="U117" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>21.745047041880969</v>
       </c>
       <c r="V117" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>21.825227893805309</v>
       </c>
       <c r="W117" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>22.21847524324324</v>
       </c>
       <c r="X117" t="s">
@@ -5424,27 +5457,27 @@
         <v>0.85599999999999998</v>
       </c>
       <c r="R118" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="S118" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="T118" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.58</v>
       </c>
       <c r="U118" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16.969615266055047</v>
       </c>
       <c r="V118" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>17.367963042253521</v>
       </c>
       <c r="W118" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>17.286804336448597</v>
       </c>
       <c r="X118" t="s">
@@ -5497,27 +5530,27 @@
         <v>0.36</v>
       </c>
       <c r="R119" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="S119" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="T119" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.427</v>
       </c>
       <c r="U119" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.9276706516853928</v>
       </c>
       <c r="V119" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6.9406681575984983</v>
       </c>
       <c r="W119" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10.276044799999999</v>
       </c>
       <c r="X119" t="s">
@@ -5570,11 +5603,11 @@
         <v>0.90200000000000002</v>
       </c>
       <c r="R120" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>112</v>
       </c>
       <c r="S120" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
       <c r="T120" s="2">
@@ -5582,14 +5615,14 @@
         <v>1.472</v>
       </c>
       <c r="U120" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.6253446736842108</v>
       </c>
       <c r="V120" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W120" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.1867477427937914</v>
       </c>
       <c r="X120" t="s">
@@ -5642,11 +5675,11 @@
         <v>0.34399999999999997</v>
       </c>
       <c r="R121" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="S121" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="T121" s="2">
@@ -5654,15 +5687,15 @@
         <v>1.8340000000000001</v>
       </c>
       <c r="U121" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.5820651605231868</v>
       </c>
       <c r="V121" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.9376221879815096</v>
       </c>
       <c r="W121" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11.202083720930235</v>
       </c>
       <c r="X121" t="s">
@@ -5715,27 +5748,27 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="R122" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="S122" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="T122" s="2">
-        <f t="shared" ref="T122:T126" si="12">N122+O122+P122</f>
+        <f t="shared" ref="T122:T126" si="14">N122+O122+P122</f>
         <v>0.29099999999999998</v>
       </c>
       <c r="U122" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.3419907605633812</v>
       </c>
       <c r="V122" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.1104179200000006</v>
       </c>
       <c r="W122" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.1260782344827587</v>
       </c>
       <c r="X122" t="s">
@@ -5788,27 +5821,27 @@
         <v>0.53800000000000003</v>
       </c>
       <c r="R123" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="S123" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="T123" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.7649999999999999</v>
       </c>
       <c r="U123" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.3820067039106156</v>
       </c>
       <c r="V123" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.5411287671232872</v>
       </c>
       <c r="W123" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.1626706319702595</v>
       </c>
       <c r="X123" t="s">
@@ -5861,27 +5894,27 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R124" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="S124" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="T124" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.40500000000000003</v>
       </c>
       <c r="U124" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.3419907605633812</v>
       </c>
       <c r="V124" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.0127047804878044</v>
       </c>
       <c r="W124" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.4040191999999996</v>
       </c>
       <c r="X124" t="s">
@@ -5934,27 +5967,27 @@
         <v>0.12</v>
       </c>
       <c r="R125" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="S125" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="T125" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.35099999999999998</v>
       </c>
       <c r="U125" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.3192462222222225</v>
       </c>
       <c r="V125" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.8387523678160917</v>
       </c>
       <c r="W125" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.783095466666667</v>
       </c>
       <c r="X125" t="s">
@@ -6007,27 +6040,27 @@
         <v>0.81399999999999995</v>
       </c>
       <c r="R126" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="S126" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="T126" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2.7090000000000001</v>
       </c>
       <c r="U126" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.6019354616048314</v>
       </c>
       <c r="V126" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.6720695652173916</v>
       </c>
       <c r="W126" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.1285542997542999</v>
       </c>
       <c r="X126" t="s">
@@ -6080,11 +6113,11 @@
       <c r="E138">
         <v>50</v>
       </c>
-      <c r="G138">
+      <c r="G138" s="2">
         <f>4422/(1000)</f>
         <v>4.4219999999999997</v>
       </c>
-      <c r="H138">
+      <c r="H138" s="2">
         <f>4036/(1000)</f>
         <v>4.0359999999999996</v>
       </c>
@@ -6107,20 +6140,20 @@
       <c r="E139">
         <v>50</v>
       </c>
-      <c r="G139">
+      <c r="G139" s="2">
         <f>13804/(1000)</f>
         <v>13.804</v>
       </c>
-      <c r="H139">
+      <c r="H139" s="2">
         <f>13254/(1000)</f>
         <v>13.254</v>
       </c>
       <c r="I139" s="2">
-        <f t="shared" ref="I139:J149" si="13">(2*$E139*$D139*$C139*$C139+$E139*$D139*$C139)/(G139/1000)/10^12</f>
+        <f t="shared" ref="I139:J149" si="15">(2*$E139*$D139*$C139*$C139+$E139*$D139*$C139)/(G139/1000)/10^12</f>
         <v>0.71827991886409726</v>
       </c>
       <c r="J139" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.74808631356571598</v>
       </c>
     </row>
@@ -6134,20 +6167,20 @@
       <c r="E140">
         <v>50</v>
       </c>
-      <c r="G140">
+      <c r="G140" s="2">
         <f>6780/(1000)</f>
         <v>6.78</v>
       </c>
-      <c r="H140">
+      <c r="H140" s="2">
         <f>6364/(1000)</f>
         <v>6.3639999999999999</v>
       </c>
       <c r="I140" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2.9248188790560468</v>
       </c>
       <c r="J140" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3.1160075424261469</v>
       </c>
     </row>
@@ -6165,20 +6198,20 @@
       <c r="E141">
         <v>50</v>
       </c>
-      <c r="G141">
+      <c r="G141" s="2">
         <f>8902/(1000)</f>
         <v>8.9019999999999992</v>
       </c>
-      <c r="H141">
+      <c r="H141" s="2">
         <f>8518/(1000)</f>
         <v>8.5180000000000007</v>
       </c>
       <c r="I141" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.4552397214109201</v>
       </c>
       <c r="J141" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.6560864052594502</v>
       </c>
     </row>
@@ -6192,20 +6225,20 @@
       <c r="E142">
         <v>50</v>
       </c>
-      <c r="G142">
+      <c r="G142" s="2">
         <f>5864/(1000)</f>
         <v>5.8639999999999999</v>
       </c>
-      <c r="H142">
+      <c r="H142" s="2">
         <f>5318/(1000)</f>
         <v>5.3179999999999996</v>
       </c>
       <c r="I142" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.1447006821282399</v>
       </c>
       <c r="J142" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.2622273034975555</v>
       </c>
     </row>
@@ -6219,20 +6252,20 @@
       <c r="E143">
         <v>50</v>
       </c>
-      <c r="G143">
+      <c r="G143" s="2">
         <f>15600/(1000)</f>
         <v>15.6</v>
       </c>
-      <c r="H143">
+      <c r="H143" s="2">
         <f>15238/(1000)</f>
         <v>15.238</v>
       </c>
       <c r="I143" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.86058010256410267</v>
       </c>
       <c r="J143" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.88102438640241509</v>
       </c>
     </row>
@@ -6246,20 +6279,20 @@
       <c r="E144">
         <v>50</v>
       </c>
-      <c r="G144">
+      <c r="G144" s="2">
         <f>8545/(1000)</f>
         <v>8.5449999999999999</v>
       </c>
-      <c r="H144">
+      <c r="H144" s="2">
         <f>8228/(1000)</f>
         <v>8.2279999999999998</v>
       </c>
       <c r="I144" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3.1422000234055001</v>
       </c>
       <c r="J144" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3.2632595041322321</v>
       </c>
     </row>
@@ -6277,20 +6310,20 @@
       <c r="E145">
         <v>50</v>
       </c>
-      <c r="G145">
+      <c r="G145" s="2">
         <f>11503/(1000)</f>
         <v>11.503</v>
       </c>
-      <c r="H145">
+      <c r="H145" s="2">
         <f>11225/(1000)</f>
         <v>11.225</v>
       </c>
       <c r="I145" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.6683646353125274</v>
       </c>
       <c r="J145" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.7839820400890867</v>
       </c>
     </row>
@@ -6304,20 +6337,20 @@
       <c r="E146">
         <v>50</v>
       </c>
-      <c r="G146">
+      <c r="G146" s="2">
         <f>7330/(1000)</f>
         <v>7.33</v>
       </c>
-      <c r="H146">
+      <c r="H146" s="2">
         <f>6463/(1000)</f>
         <v>6.4630000000000001</v>
       </c>
       <c r="I146" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.430806002728513</v>
       </c>
       <c r="J146" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.6227460931455979</v>
       </c>
     </row>
@@ -6331,20 +6364,20 @@
       <c r="E147">
         <v>50</v>
       </c>
-      <c r="G147">
+      <c r="G147" s="2">
         <f>18959/(1000)</f>
         <v>18.959</v>
       </c>
-      <c r="H147">
+      <c r="H147" s="2">
         <f>18428/(1000)</f>
         <v>18.428000000000001</v>
       </c>
       <c r="I147" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.1063672134606255</v>
       </c>
       <c r="J147" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.1382470154113307</v>
       </c>
     </row>
@@ -6358,20 +6391,20 @@
       <c r="E148">
         <v>50</v>
       </c>
-      <c r="G148">
+      <c r="G148" s="2">
         <f>8933/(1000)</f>
         <v>8.9329999999999998</v>
       </c>
-      <c r="H148">
+      <c r="H148" s="2">
         <f>8491/(1000)</f>
         <v>8.4909999999999997</v>
       </c>
       <c r="I148" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.6962086645024073</v>
       </c>
       <c r="J148" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.940670356848428</v>
       </c>
     </row>
@@ -6385,22 +6418,34 @@
       <c r="E149">
         <v>50</v>
       </c>
-      <c r="G149">
+      <c r="G149" s="2">
         <f>14373/(1000)</f>
         <v>14.372999999999999</v>
       </c>
-      <c r="H149">
+      <c r="H149" s="2">
         <f>14411/(1000)</f>
         <v>14.411</v>
       </c>
       <c r="I149" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>5.8375053224796494</v>
       </c>
       <c r="J149" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>5.822112552910971</v>
       </c>
+    </row>
+    <row r="150" spans="1:10">
+      <c r="G150" s="2"/>
+      <c r="H150" s="2"/>
+    </row>
+    <row r="151" spans="1:10">
+      <c r="G151" s="2"/>
+      <c r="H151" s="2"/>
+    </row>
+    <row r="152" spans="1:10">
+      <c r="G152" s="2"/>
+      <c r="H152" s="2"/>
     </row>
     <row r="153" spans="1:10">
       <c r="A153" t="s">
@@ -6415,10 +6460,10 @@
       <c r="E153" t="s">
         <v>16</v>
       </c>
-      <c r="G153" t="s">
+      <c r="G153" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H153" t="s">
+      <c r="H153" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I153" t="s">
@@ -6438,20 +6483,20 @@
       <c r="E154">
         <v>25</v>
       </c>
-      <c r="G154">
+      <c r="G154" s="2">
         <f>1420/(1000)</f>
         <v>1.42</v>
       </c>
-      <c r="H154">
+      <c r="H154" s="2">
         <f>1818/(1000)</f>
         <v>1.8180000000000001</v>
       </c>
       <c r="I154" s="2">
-        <f t="shared" ref="I154:I169" si="14">(8*$E154*$D154*$C154*$C154)/(G154/1000)/10^12</f>
+        <f t="shared" ref="I154:I169" si="16">(8*$E154*$D154*$C154*$C154)/(G154/1000)/10^12</f>
         <v>0.59074704225352126</v>
       </c>
       <c r="J154" s="2">
-        <f t="shared" ref="J154:J169" si="15">(8*$E154*$D154*$C154*$C154)/(H154/1000)/10^12</f>
+        <f t="shared" ref="J154:J169" si="17">(8*$E154*$D154*$C154*$C154)/(H154/1000)/10^12</f>
         <v>0.46141958195819582</v>
       </c>
     </row>
@@ -6465,20 +6510,20 @@
       <c r="E155">
         <v>25</v>
       </c>
-      <c r="G155">
+      <c r="G155" s="2">
         <f>2926/(1000)</f>
         <v>2.9260000000000002</v>
       </c>
-      <c r="H155">
+      <c r="H155" s="2">
         <f>7460/(1000)</f>
         <v>7.46</v>
       </c>
       <c r="I155" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.573384005468216</v>
       </c>
       <c r="J155" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.22489565683646115</v>
       </c>
     </row>
@@ -6492,20 +6537,20 @@
       <c r="E156">
         <v>25</v>
       </c>
-      <c r="G156">
+      <c r="G156" s="2">
         <f>2955/(1000)</f>
         <v>2.9550000000000001</v>
       </c>
-      <c r="H156">
+      <c r="H156" s="2">
         <f>3030/(1000)</f>
         <v>3.03</v>
       </c>
       <c r="I156" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.1355137732656513</v>
       </c>
       <c r="J156" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.1074069966996702</v>
       </c>
     </row>
@@ -6519,20 +6564,20 @@
       <c r="E157">
         <v>25</v>
       </c>
-      <c r="G157">
+      <c r="G157" s="2">
         <f>3164/(1000)</f>
         <v>3.1640000000000001</v>
       </c>
-      <c r="H157">
+      <c r="H157" s="2">
         <f>3206/(1000)</f>
         <v>3.206</v>
       </c>
       <c r="I157" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2.1210134007585335</v>
       </c>
       <c r="J157" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2.0932271990018712</v>
       </c>
     </row>
@@ -6546,20 +6591,20 @@
       <c r="E158">
         <v>25</v>
       </c>
-      <c r="G158">
+      <c r="G158" s="2">
         <f>3471/(1000)</f>
         <v>3.4710000000000001</v>
       </c>
-      <c r="H158">
+      <c r="H158" s="2">
         <f>3103/(1000)</f>
         <v>3.1030000000000002</v>
       </c>
       <c r="I158" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.96670792278882167</v>
       </c>
       <c r="J158" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.0813545601031258</v>
       </c>
     </row>
@@ -6573,20 +6618,20 @@
       <c r="E159">
         <v>25</v>
       </c>
-      <c r="G159">
+      <c r="G159" s="2">
         <f>4908/(1000)</f>
         <v>4.9080000000000004</v>
       </c>
-      <c r="H159">
+      <c r="H159" s="2">
         <f>13803/(1000)</f>
         <v>13.803000000000001</v>
       </c>
       <c r="I159" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.3673362673186633</v>
       </c>
       <c r="J159" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.48619042237194809</v>
       </c>
     </row>
@@ -6600,24 +6645,24 @@
       <c r="E160">
         <v>25</v>
       </c>
-      <c r="G160">
+      <c r="G160" s="2">
         <f>4823/(1000)</f>
         <v>4.8230000000000004</v>
       </c>
-      <c r="H160">
+      <c r="H160" s="2">
         <f>4655/(1000)</f>
         <v>4.6550000000000002</v>
       </c>
       <c r="I160" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2.7828680904001661</v>
       </c>
       <c r="J160" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2.8833024274973145</v>
       </c>
     </row>
-    <row r="161" spans="3:10">
+    <row r="161" spans="1:11">
       <c r="C161">
         <v>1024</v>
       </c>
@@ -6627,24 +6672,24 @@
       <c r="E161">
         <v>25</v>
       </c>
-      <c r="G161">
+      <c r="G161" s="2">
         <f>7233/(1000)</f>
         <v>7.2329999999999997</v>
       </c>
-      <c r="H161">
+      <c r="H161" s="2">
         <f>6228/(1000)</f>
         <v>6.2279999999999998</v>
       </c>
       <c r="I161" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>3.7112602792755429</v>
       </c>
       <c r="J161" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4.3101389852280025</v>
       </c>
     </row>
-    <row r="162" spans="3:10">
+    <row r="162" spans="1:11">
       <c r="C162">
         <v>2048</v>
       </c>
@@ -6654,24 +6699,24 @@
       <c r="E162">
         <v>25</v>
       </c>
-      <c r="G162">
+      <c r="G162" s="2">
         <f>12862/(1000)</f>
         <v>12.862</v>
       </c>
-      <c r="H162">
+      <c r="H162" s="2">
         <f>9701/(1000)</f>
         <v>9.7010000000000005</v>
       </c>
       <c r="I162" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0435214430104183</v>
       </c>
       <c r="J162" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.3835452839913409</v>
       </c>
     </row>
-    <row r="163" spans="3:10">
+    <row r="163" spans="1:11">
       <c r="C163">
         <v>2048</v>
       </c>
@@ -6681,24 +6726,24 @@
       <c r="E163">
         <v>25</v>
       </c>
-      <c r="G163">
+      <c r="G163" s="2">
         <f>9477/(1000)</f>
         <v>9.4770000000000003</v>
       </c>
-      <c r="H163">
+      <c r="H163" s="2">
         <f>26948/(1000)</f>
         <v>26.948</v>
       </c>
       <c r="I163" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2.8324939959902919</v>
       </c>
       <c r="J163" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.99612385334718712</v>
       </c>
     </row>
-    <row r="164" spans="3:10">
+    <row r="164" spans="1:11">
       <c r="C164">
         <v>2048</v>
       </c>
@@ -6708,24 +6753,24 @@
       <c r="E164">
         <v>25</v>
       </c>
-      <c r="G164">
+      <c r="G164" s="2">
         <f>11700/(1000)</f>
         <v>11.7</v>
       </c>
-      <c r="H164">
+      <c r="H164" s="2">
         <f>9659/(1000)</f>
         <v>9.6590000000000007</v>
       </c>
       <c r="I164" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4.5886402735042742</v>
       </c>
       <c r="J164" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5.5582452841909094</v>
       </c>
     </row>
-    <row r="165" spans="3:10">
+    <row r="165" spans="1:11">
       <c r="C165">
         <v>2048</v>
       </c>
@@ -6735,24 +6780,24 @@
       <c r="E165">
         <v>25</v>
       </c>
-      <c r="G165">
+      <c r="G165" s="2">
         <f>23163/(1000)</f>
         <v>23.163</v>
       </c>
-      <c r="H165">
+      <c r="H165" s="2">
         <f>16065/(1000)</f>
         <v>16.065000000000001</v>
       </c>
       <c r="I165" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4.6355904848249363</v>
       </c>
       <c r="J165" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6.6837337317149075</v>
       </c>
     </row>
-    <row r="166" spans="3:10">
+    <row r="166" spans="1:11">
       <c r="C166">
         <v>4096</v>
       </c>
@@ -6762,24 +6807,24 @@
       <c r="E166">
         <v>25</v>
       </c>
-      <c r="G166">
+      <c r="G166" s="2">
         <f>50641/(1000)</f>
         <v>50.640999999999998</v>
       </c>
-      <c r="H166">
+      <c r="H166" s="2">
         <f>46550/(1000)</f>
         <v>46.55</v>
       </c>
       <c r="I166" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0601506921269328</v>
       </c>
       <c r="J166" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.1533209709989261</v>
       </c>
     </row>
-    <row r="167" spans="3:10">
+    <row r="167" spans="1:11">
       <c r="C167">
         <v>4096</v>
       </c>
@@ -6789,24 +6834,24 @@
       <c r="E167">
         <v>25</v>
       </c>
-      <c r="G167">
+      <c r="G167" s="2">
         <f>22638/(1000)</f>
         <v>22.638000000000002</v>
       </c>
-      <c r="H167">
+      <c r="H167" s="2">
         <f>56440/(1000)</f>
         <v>56.44</v>
       </c>
       <c r="I167" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4.7430949023765345</v>
       </c>
       <c r="J167" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.9024483061658399</v>
       </c>
     </row>
-    <row r="168" spans="3:10">
+    <row r="168" spans="1:11">
       <c r="C168">
         <v>4096</v>
       </c>
@@ -6816,24 +6861,24 @@
       <c r="E168">
         <v>25</v>
       </c>
-      <c r="G168">
+      <c r="G168" s="2">
         <f>34880/(1000)</f>
         <v>34.880000000000003</v>
       </c>
-      <c r="H168">
+      <c r="H168" s="2">
         <f>59547/(1000)</f>
         <v>59.546999999999997</v>
       </c>
       <c r="I168" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>6.1567765137614678</v>
       </c>
       <c r="J168" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3.6063674878667276</v>
       </c>
     </row>
-    <row r="169" spans="3:10">
+    <row r="169" spans="1:11">
       <c r="C169">
         <v>4096</v>
       </c>
@@ -6843,26 +6888,630 @@
       <c r="E169">
         <v>25</v>
       </c>
-      <c r="G169">
+      <c r="G169" s="2">
         <f>67436/(1000)</f>
         <v>67.436000000000007</v>
       </c>
-      <c r="H169">
+      <c r="H169" s="2">
         <f>54918/(1000)</f>
         <v>54.917999999999999</v>
       </c>
       <c r="I169" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>6.3689532237973774</v>
       </c>
       <c r="J169" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>7.8206913871590373</v>
       </c>
     </row>
-    <row r="172" spans="3:10">
+    <row r="172" spans="1:11">
       <c r="G172" s="2"/>
       <c r="H172" s="2"/>
+    </row>
+    <row r="173" spans="1:11">
+      <c r="A173" t="s">
+        <v>66</v>
+      </c>
+      <c r="C173" t="s">
+        <v>67</v>
+      </c>
+      <c r="D173" t="s">
+        <v>68</v>
+      </c>
+      <c r="G173" t="s">
+        <v>69</v>
+      </c>
+      <c r="I173" t="s">
+        <v>70</v>
+      </c>
+      <c r="J173" t="s">
+        <v>71</v>
+      </c>
+      <c r="K173" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11">
+      <c r="C175">
+        <v>100000</v>
+      </c>
+      <c r="D175">
+        <v>2</v>
+      </c>
+      <c r="G175" s="2">
+        <v>6.1183596078431372E-2</v>
+      </c>
+      <c r="H175" s="2"/>
+      <c r="I175" s="2">
+        <f>C175*4*D175/(G175/1000)/10^9</f>
+        <v>13.075400128074826</v>
+      </c>
+      <c r="J175" t="s">
+        <v>76</v>
+      </c>
+      <c r="K175" s="2">
+        <v>1.5088436641296915E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11">
+      <c r="C176">
+        <v>100000</v>
+      </c>
+      <c r="D176">
+        <v>4</v>
+      </c>
+      <c r="G176" s="2">
+        <v>8.9482190196078434E-2</v>
+      </c>
+      <c r="H176" s="2"/>
+      <c r="I176" s="2">
+        <f t="shared" ref="I176:I199" si="18">C176*4*D176/(G176/1000)/10^9</f>
+        <v>17.880653082965331</v>
+      </c>
+      <c r="J176" t="s">
+        <v>76</v>
+      </c>
+      <c r="K176" s="2">
+        <v>1.1876097542972443E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="3:11">
+      <c r="C177">
+        <v>100000</v>
+      </c>
+      <c r="D177">
+        <v>8</v>
+      </c>
+      <c r="G177" s="2">
+        <v>0.21871601960784315</v>
+      </c>
+      <c r="H177" s="2"/>
+      <c r="I177" s="2">
+        <f t="shared" si="18"/>
+        <v>14.630844168331089</v>
+      </c>
+      <c r="J177" t="s">
+        <v>76</v>
+      </c>
+      <c r="K177" s="2">
+        <v>4.5119592573080536E-3</v>
+      </c>
+    </row>
+    <row r="178" spans="3:11">
+      <c r="C178">
+        <v>100000</v>
+      </c>
+      <c r="D178">
+        <v>16</v>
+      </c>
+      <c r="E178">
+        <v>2</v>
+      </c>
+      <c r="G178" s="2">
+        <v>0.62921153846153832</v>
+      </c>
+      <c r="I178" s="2">
+        <f t="shared" si="18"/>
+        <v>10.171460007946456</v>
+      </c>
+      <c r="J178" t="s">
+        <v>74</v>
+      </c>
+      <c r="K178" s="2">
+        <v>3.9179270507992622E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="3:11">
+      <c r="C179">
+        <v>100000</v>
+      </c>
+      <c r="D179">
+        <v>32</v>
+      </c>
+      <c r="E179">
+        <v>4</v>
+      </c>
+      <c r="G179" s="2">
+        <v>0.79834720000000003</v>
+      </c>
+      <c r="I179" s="2">
+        <f t="shared" si="18"/>
+        <v>16.033124435082883</v>
+      </c>
+      <c r="J179" t="s">
+        <v>74</v>
+      </c>
+      <c r="K179" s="2">
+        <v>4.5644606337076302E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="3:11">
+      <c r="C180">
+        <v>3097600</v>
+      </c>
+      <c r="D180">
+        <v>2</v>
+      </c>
+      <c r="G180" s="2">
+        <v>1.0749607843137254</v>
+      </c>
+      <c r="H180" s="2"/>
+      <c r="I180" s="2">
+        <f t="shared" si="18"/>
+        <v>23.052747934261166</v>
+      </c>
+      <c r="J180" t="s">
+        <v>73</v>
+      </c>
+      <c r="K180" s="2">
+        <v>1.0749607843137254</v>
+      </c>
+    </row>
+    <row r="181" spans="3:11">
+      <c r="C181">
+        <f>1760*1760</f>
+        <v>3097600</v>
+      </c>
+      <c r="D181">
+        <v>4</v>
+      </c>
+      <c r="G181" s="2">
+        <v>2.1395686274509802</v>
+      </c>
+      <c r="H181" s="2"/>
+      <c r="I181" s="2">
+        <f t="shared" si="18"/>
+        <v>23.164295533275904</v>
+      </c>
+      <c r="J181" t="s">
+        <v>73</v>
+      </c>
+      <c r="K181" s="2">
+        <v>2.1395686274509802</v>
+      </c>
+    </row>
+    <row r="182" spans="3:11">
+      <c r="C182">
+        <f>1760*1760</f>
+        <v>3097600</v>
+      </c>
+      <c r="D182">
+        <v>8</v>
+      </c>
+      <c r="G182" s="2">
+        <v>4.2866078431372543</v>
+      </c>
+      <c r="H182" s="2"/>
+      <c r="I182" s="2">
+        <f t="shared" si="18"/>
+        <v>23.123925403788366</v>
+      </c>
+      <c r="J182" t="s">
+        <v>73</v>
+      </c>
+      <c r="K182" s="2">
+        <v>4.2866078431372543</v>
+      </c>
+    </row>
+    <row r="183" spans="3:11">
+      <c r="C183">
+        <v>3097600</v>
+      </c>
+      <c r="D183">
+        <v>16</v>
+      </c>
+      <c r="E183">
+        <v>2</v>
+      </c>
+      <c r="G183" s="2">
+        <v>21.871352307692312</v>
+      </c>
+      <c r="I183" s="2">
+        <f t="shared" si="18"/>
+        <v>9.0642040423936354</v>
+      </c>
+      <c r="J183" t="s">
+        <v>75</v>
+      </c>
+      <c r="K183" s="2">
+        <v>1.7163970672552604</v>
+      </c>
+    </row>
+    <row r="184" spans="3:11">
+      <c r="C184">
+        <v>3097600</v>
+      </c>
+      <c r="D184">
+        <v>32</v>
+      </c>
+      <c r="E184">
+        <v>4</v>
+      </c>
+      <c r="G184" s="2">
+        <v>21.651951600000004</v>
+      </c>
+      <c r="I184" s="2">
+        <f t="shared" si="18"/>
+        <v>18.312104484844681</v>
+      </c>
+      <c r="J184" t="s">
+        <v>75</v>
+      </c>
+      <c r="K184" s="2">
+        <v>1.4565773319488855</v>
+      </c>
+    </row>
+    <row r="185" spans="3:11">
+      <c r="C185">
+        <v>4194304</v>
+      </c>
+      <c r="D185">
+        <v>2</v>
+      </c>
+      <c r="G185" s="2">
+        <v>1.4430392156862746</v>
+      </c>
+      <c r="H185" s="2"/>
+      <c r="I185" s="2">
+        <f t="shared" si="18"/>
+        <v>23.252612704667435</v>
+      </c>
+      <c r="J185" t="s">
+        <v>73</v>
+      </c>
+      <c r="K185" s="2">
+        <v>2.1905322121687845E-3</v>
+      </c>
+    </row>
+    <row r="186" spans="3:11">
+      <c r="C186">
+        <f>2048*2048</f>
+        <v>4194304</v>
+      </c>
+      <c r="D186">
+        <v>4</v>
+      </c>
+      <c r="G186" s="2">
+        <v>2.8808823529411756</v>
+      </c>
+      <c r="H186" s="2"/>
+      <c r="I186" s="2">
+        <f t="shared" si="18"/>
+        <v>23.294552077590616</v>
+      </c>
+      <c r="J186" t="s">
+        <v>73</v>
+      </c>
+      <c r="K186" s="2">
+        <v>3.947895939983884E-3</v>
+      </c>
+    </row>
+    <row r="187" spans="3:11">
+      <c r="C187">
+        <f>2048*2048</f>
+        <v>4194304</v>
+      </c>
+      <c r="D187">
+        <v>8</v>
+      </c>
+      <c r="G187" s="2">
+        <v>5.7344901960784318</v>
+      </c>
+      <c r="H187" s="2"/>
+      <c r="I187" s="2">
+        <f t="shared" si="18"/>
+        <v>23.405346144245858</v>
+      </c>
+      <c r="J187" t="s">
+        <v>73</v>
+      </c>
+      <c r="K187" s="2">
+        <v>9.3323603134259595E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="3:11">
+      <c r="C188">
+        <v>4194304</v>
+      </c>
+      <c r="D188">
+        <v>16</v>
+      </c>
+      <c r="E188">
+        <v>2</v>
+      </c>
+      <c r="G188" s="2">
+        <v>26.65080961538462</v>
+      </c>
+      <c r="I188" s="2">
+        <f t="shared" si="18"/>
+        <v>10.072318997957991</v>
+      </c>
+      <c r="J188" t="s">
+        <v>75</v>
+      </c>
+      <c r="K188" s="2">
+        <v>2.7562195316374325</v>
+      </c>
+    </row>
+    <row r="189" spans="3:11">
+      <c r="C189">
+        <v>4194304</v>
+      </c>
+      <c r="D189">
+        <v>32</v>
+      </c>
+      <c r="E189">
+        <v>4</v>
+      </c>
+      <c r="G189" s="2">
+        <v>26.922246399999999</v>
+      </c>
+      <c r="I189" s="2">
+        <f t="shared" si="18"/>
+        <v>19.941534745035245</v>
+      </c>
+      <c r="J189" t="s">
+        <v>75</v>
+      </c>
+      <c r="K189" s="2">
+        <v>2.0811969772142342</v>
+      </c>
+    </row>
+    <row r="190" spans="3:11">
+      <c r="C190">
+        <v>6553600</v>
+      </c>
+      <c r="D190">
+        <v>2</v>
+      </c>
+      <c r="G190" s="2">
+        <v>2.2364509803921568</v>
+      </c>
+      <c r="H190" s="2"/>
+      <c r="I190" s="2">
+        <f t="shared" si="18"/>
+        <v>23.44285676711176</v>
+      </c>
+      <c r="J190" t="s">
+        <v>73</v>
+      </c>
+      <c r="K190" s="2">
+        <v>2.7879291633052653E-3</v>
+      </c>
+    </row>
+    <row r="191" spans="3:11">
+      <c r="C191">
+        <f>2560*2560</f>
+        <v>6553600</v>
+      </c>
+      <c r="D191">
+        <v>4</v>
+      </c>
+      <c r="G191" s="2">
+        <v>4.4831372549019601</v>
+      </c>
+      <c r="H191" s="2"/>
+      <c r="I191" s="2">
+        <f t="shared" si="18"/>
+        <v>23.389335199440172</v>
+      </c>
+      <c r="J191" t="s">
+        <v>73</v>
+      </c>
+      <c r="K191" s="2">
+        <v>7.2000544660249096E-3</v>
+      </c>
+    </row>
+    <row r="192" spans="3:11">
+      <c r="C192">
+        <f>2560*2560</f>
+        <v>6553600</v>
+      </c>
+      <c r="D192">
+        <v>8</v>
+      </c>
+      <c r="G192" s="2">
+        <v>8.9875098039215668</v>
+      </c>
+      <c r="H192" s="2"/>
+      <c r="I192" s="2">
+        <f t="shared" si="18"/>
+        <v>23.334071903709507</v>
+      </c>
+      <c r="J192" t="s">
+        <v>73</v>
+      </c>
+      <c r="K192" s="2">
+        <v>0.10592834796201038</v>
+      </c>
+    </row>
+    <row r="193" spans="3:11">
+      <c r="C193">
+        <v>6553600</v>
+      </c>
+      <c r="D193">
+        <v>16</v>
+      </c>
+      <c r="E193">
+        <v>2</v>
+      </c>
+      <c r="G193" s="2">
+        <v>39.265769230769237</v>
+      </c>
+      <c r="I193" s="2">
+        <f t="shared" si="18"/>
+        <v>10.681833266399584</v>
+      </c>
+      <c r="J193" t="s">
+        <v>75</v>
+      </c>
+      <c r="K193" s="2">
+        <v>2.5073686109161102</v>
+      </c>
+    </row>
+    <row r="194" spans="3:11">
+      <c r="C194">
+        <v>6553600</v>
+      </c>
+      <c r="D194">
+        <v>32</v>
+      </c>
+      <c r="E194">
+        <v>4</v>
+      </c>
+      <c r="G194" s="2">
+        <v>42.322568799999992</v>
+      </c>
+      <c r="I194" s="2">
+        <f t="shared" si="18"/>
+        <v>19.820649449803717</v>
+      </c>
+      <c r="J194" t="s">
+        <v>75</v>
+      </c>
+      <c r="K194" s="2">
+        <v>3.012434393884952</v>
+      </c>
+    </row>
+    <row r="195" spans="3:11">
+      <c r="C195">
+        <f t="shared" ref="C195:C197" si="19">4096*4096</f>
+        <v>16777216</v>
+      </c>
+      <c r="D195">
+        <v>2</v>
+      </c>
+      <c r="G195" s="2">
+        <v>5.6760392156862736</v>
+      </c>
+      <c r="H195" s="2"/>
+      <c r="I195" s="2">
+        <f t="shared" si="18"/>
+        <v>23.646370805380727</v>
+      </c>
+      <c r="J195" t="s">
+        <v>73</v>
+      </c>
+      <c r="K195" s="2">
+        <v>2.8210691896068374E-3</v>
+      </c>
+    </row>
+    <row r="196" spans="3:11">
+      <c r="C196">
+        <f t="shared" si="19"/>
+        <v>16777216</v>
+      </c>
+      <c r="D196">
+        <v>4</v>
+      </c>
+      <c r="G196" s="2">
+        <v>11.485274509803922</v>
+      </c>
+      <c r="H196" s="2"/>
+      <c r="I196" s="2">
+        <f t="shared" si="18"/>
+        <v>23.372141063834512</v>
+      </c>
+      <c r="J196" t="s">
+        <v>73</v>
+      </c>
+      <c r="K196" s="2">
+        <v>1.1636285371840076E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="3:11">
+      <c r="C197">
+        <f t="shared" si="19"/>
+        <v>16777216</v>
+      </c>
+      <c r="D197">
+        <v>8</v>
+      </c>
+      <c r="G197" s="2">
+        <v>22.924705882352942</v>
+      </c>
+      <c r="H197" s="2"/>
+      <c r="I197" s="2">
+        <f t="shared" si="18"/>
+        <v>23.418878948989018</v>
+      </c>
+      <c r="J197" t="s">
+        <v>73</v>
+      </c>
+      <c r="K197" s="2">
+        <v>0.23232195712998352</v>
+      </c>
+    </row>
+    <row r="198" spans="3:11">
+      <c r="C198">
+        <v>16777216</v>
+      </c>
+      <c r="D198">
+        <v>16</v>
+      </c>
+      <c r="E198">
+        <v>2</v>
+      </c>
+      <c r="G198" s="2">
+        <v>101.75970461538462</v>
+      </c>
+      <c r="H198" s="2"/>
+      <c r="I198" s="2">
+        <f t="shared" si="18"/>
+        <v>10.551738805240847</v>
+      </c>
+      <c r="J198" t="s">
+        <v>75</v>
+      </c>
+      <c r="K198" s="2">
+        <v>5.5600189762476386</v>
+      </c>
+    </row>
+    <row r="199" spans="3:11">
+      <c r="C199">
+        <v>16777216</v>
+      </c>
+      <c r="D199">
+        <v>32</v>
+      </c>
+      <c r="E199">
+        <v>4</v>
+      </c>
+      <c r="G199" s="2">
+        <v>108.21256479999998</v>
+      </c>
+      <c r="H199" s="2"/>
+      <c r="I199" s="2">
+        <f t="shared" si="18"/>
+        <v>19.845048973462649</v>
+      </c>
+      <c r="J199" t="s">
+        <v>75</v>
+      </c>
+      <c r="K199" s="2">
+        <v>9.0259494651879173</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>